<commit_message>
Updated design notes for the outcome definitions.
</commit_message>
<xml_diff>
--- a/vignettes/OpioidUse_UDS_Variables_20210422.xlsx
+++ b/vignettes/OpioidUse_UDS_Variables_20210422.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/CTN-0094/CTNote/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D51A6FA-FF3B-1348-8252-5B55B514F970}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CD7B1D-2688-A342-ADC1-099FB742752A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{486588A9-6F67-4D40-8009-2F993698A2A4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
   <si>
     <t>Primary Endpoint</t>
   </si>
@@ -222,7 +222,55 @@
     <t>These complete abstinence metrics only change their behaviour with respect to how missing UDS are treated. For this metric, missings are allowed, so long as we have 6 months (10 - 4) of negative monthly UDS</t>
   </si>
   <si>
-    <t xml:space="preserve">I'd need to create a function that allows the user to specifically check certain </t>
+    <t>I'd need to create a function that allows the user to specifically check certain weeks / dates (indicies?) of the timeline and count failures for those dates only. But how do we handle missingness? If the dates of observation are fixed, missings should be counted as positive.</t>
+  </si>
+  <si>
+    <t>This is just a count of all the negative UDS, right? But we still have to check "weeks" because we don't want two negative UDS in one week to count as a 2.</t>
+  </si>
+  <si>
+    <t>TimeToOutcome</t>
+  </si>
+  <si>
+    <t>TimeToOutcome uses the proportion calculated by AddFailCounts(), so we would set this count to 1 to mark each positive or missing UDS as a single failure. This means that we can probably use TimeToOutcome() for all sorts of events, as long as some other function codes what that event is.</t>
+  </si>
+  <si>
+    <t>I know that Sean says the failure date should be marked as D - 3 if the third consecutive failure happens on day D. However, in practice, this is impossible without a time machine. Perhaps we can add an argument that allows us to mark the start or the end of the interval as the time of failure.</t>
+  </si>
+  <si>
+    <t>Again, are missing UDS a sign of use? This should be an argument.</t>
+  </si>
+  <si>
+    <t>This on might require a custom definition. Or perhaps we should change the scale from weekly to daily (we would really want those for() loops in C)? Then, we can assign weights to positive and negative UDS taken weekly, and also account for this "missing = +5" thing.</t>
+  </si>
+  <si>
+    <t>time to first positive or missing</t>
+  </si>
+  <si>
+    <t>Again, start or end of the interval? Also, we probably need to code up functions to deal with self-report data. I just don't trust that data at all.</t>
+  </si>
+  <si>
+    <t>Interesting. But I think it makes sense to do this by day, to avoid the edge cases of a person coming in on Monday and Saturday of the same week.</t>
+  </si>
+  <si>
+    <t>What about missing?</t>
+  </si>
+  <si>
+    <t>This is just a proportion in a window, but the window is at the end of treatment.</t>
+  </si>
+  <si>
+    <t>nFails would be set to 48?</t>
+  </si>
+  <si>
+    <t>What is a success?</t>
+  </si>
+  <si>
+    <t>nFails = 24-5 = 19?</t>
+  </si>
+  <si>
+    <t>nFails = 12</t>
+  </si>
+  <si>
+    <t>This would also be that function where the user specifies the exact days to count UDS.</t>
   </si>
 </sst>
 </file>
@@ -591,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0730C9FF-B84E-414F-BE33-3EEBF943F5F1}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,8 +648,8 @@
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="138.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="236" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="247.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -749,6 +797,9 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -760,6 +811,9 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -771,6 +825,12 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -782,6 +842,12 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -793,6 +859,12 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -804,8 +876,11 @@
       <c r="C15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -815,8 +890,14 @@
       <c r="C16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -826,8 +907,11 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -837,8 +921,11 @@
       <c r="C18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -848,8 +935,11 @@
       <c r="C19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -859,8 +949,14 @@
       <c r="C20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -870,8 +966,14 @@
       <c r="C21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -881,8 +983,11 @@
       <c r="C22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -892,8 +997,11 @@
       <c r="C23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -903,8 +1011,11 @@
       <c r="C24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -914,8 +1025,14 @@
       <c r="C25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -925,8 +1042,11 @@
       <c r="C26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -936,8 +1056,14 @@
       <c r="C27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -946,6 +1072,9 @@
       </c>
       <c r="C28" t="s">
         <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More updates to Laura's table
</commit_message>
<xml_diff>
--- a/vignettes/OpioidUse_UDS_Variables_20210422.xlsx
+++ b/vignettes/OpioidUse_UDS_Variables_20210422.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/CTN-0094/CTNote/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DE2387-A2FA-6B4A-96BB-AB6C5AE08BA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CA86F1-B72D-5B4E-9888-E53C5EBCCCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{486588A9-6F67-4D40-8009-2F993698A2A4}"/>
+    <workbookView xWindow="860" yWindow="880" windowWidth="31280" windowHeight="17440" xr2:uid="{486588A9-6F67-4D40-8009-2F993698A2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,9 +264,6 @@
     <t>Mokri et al. (2016)</t>
   </si>
   <si>
-    <t>Participant has used non-protocol prescribed opioids starting at day 21 post-randomization as follows: 4 consecutive opioid use weeks OR 7 consecutive days of use by self-report. Use week: Any week during which a participant self-reports at least one day of non-prescribed opioid use, provides a urine sample positive for non-study opioids, or fails to provide a urine sample at the weekly assessment visit.</t>
-  </si>
-  <si>
     <t>Lee et al. (2018)</t>
   </si>
   <si>
@@ -343,13 +340,16 @@
   </si>
   <si>
     <t>Missingness is handled in pre-processing. Time to event can be handled with dplyr lead() / lag()</t>
+  </si>
+  <si>
+    <t>Weeks to relapse (starting at day 21 post-randomization: 4 consecutive weeks with positive UOS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,13 +372,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -393,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -403,6 +416,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0730C9FF-B84E-414F-BE33-3EEBF943F5F1}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,7 +770,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -788,7 +804,7 @@
         <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -805,7 +821,7 @@
         <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -825,7 +841,7 @@
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -842,7 +858,7 @@
         <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -862,7 +878,7 @@
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -882,7 +898,7 @@
         <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -902,7 +918,7 @@
         <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -930,7 +946,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -967,7 +983,7 @@
         <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -987,7 +1003,7 @@
         <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1007,7 +1023,7 @@
         <v>53</v>
       </c>
       <c r="G15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1047,15 +1063,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
         <v>76</v>
-      </c>
-      <c r="C18" t="s">
-        <v>77</v>
       </c>
       <c r="D18" t="s">
         <v>19</v>
@@ -1096,11 +1112,11 @@
       <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
         <v>39</v>
@@ -1114,10 +1130,10 @@
         <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s">
         <v>78</v>
-      </c>
-      <c r="C22" t="s">
-        <v>79</v>
       </c>
       <c r="D22" t="s">
         <v>35</v>
@@ -1134,10 +1150,10 @@
         <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
         <v>80</v>
-      </c>
-      <c r="C23" t="s">
-        <v>81</v>
       </c>
       <c r="D23" t="s">
         <v>35</v>
@@ -1151,10 +1167,10 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
         <v>82</v>
-      </c>
-      <c r="C24" t="s">
-        <v>83</v>
       </c>
       <c r="D24" t="s">
         <v>35</v>
@@ -1167,11 +1183,11 @@
       <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
         <v>84</v>
-      </c>
-      <c r="C25" t="s">
-        <v>85</v>
       </c>
       <c r="D25" t="s">
         <v>35</v>
@@ -1185,10 +1201,10 @@
         <v>34</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
         <v>86</v>
-      </c>
-      <c r="C26" t="s">
-        <v>87</v>
       </c>
       <c r="D26" t="s">
         <v>35</v>
@@ -1205,7 +1221,7 @@
         <v>34</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
         <v>71</v>
@@ -1222,10 +1238,10 @@
         <v>34</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
         <v>89</v>
-      </c>
-      <c r="C28" t="s">
-        <v>90</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
@@ -1242,10 +1258,10 @@
         <v>34</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s">
         <v>91</v>
-      </c>
-      <c r="C29" t="s">
-        <v>92</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>

</xml_diff>